<commit_message>
revise script and test
</commit_message>
<xml_diff>
--- a/test_files/Geriscript invoice.xlsx
+++ b/test_files/Geriscript invoice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>FacName</t>
   </si>
@@ -88,79 +88,25 @@
     <t>F</t>
   </si>
   <si>
-    <t>FARKAS,ATTILA</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>W</t>
   </si>
   <si>
-    <t>OTC</t>
-  </si>
-  <si>
     <t>FACI</t>
-  </si>
-  <si>
-    <t>MCD</t>
   </si>
   <si>
     <t>RX</t>
   </si>
   <si>
-    <t>121508</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>59762372103</t>
-  </si>
-  <si>
-    <t>ALPRAZolam 1MG TABLET</t>
-  </si>
-  <si>
-    <t>09/29/20 ASHLEY: NO OVERRIDE BY INS, SENT IN GOOD FAITH, BILLED FACI</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>BERY  @,SEEMA</t>
   </si>
   <si>
     <t>MCR</t>
-  </si>
-  <si>
-    <t>HMO</t>
-  </si>
-  <si>
-    <t>121506</t>
-  </si>
-  <si>
-    <t>520</t>
-  </si>
-  <si>
-    <t>16729002301</t>
-  </si>
-  <si>
-    <t>BICALUTAMIDE TAB 50MG</t>
-  </si>
-  <si>
-    <t>109452</t>
-  </si>
-  <si>
-    <t>523</t>
-  </si>
-  <si>
-    <t>35046000433</t>
-  </si>
-  <si>
-    <t>CO-ENZYME Q-10 200MG CAPSULES</t>
   </si>
   <si>
     <t>HMO PER DIEM</t>
@@ -172,9 +118,6 @@
     <t>HMOPD</t>
   </si>
   <si>
-    <t>From 09/01/2020 Covering 24 Days</t>
-  </si>
-  <si>
     <t>120432</t>
   </si>
   <si>
@@ -184,16 +127,7 @@
     <t>From 09/09/2020 Covering 22 Days</t>
   </si>
   <si>
-    <t>From 09/22/2020 Covering 9 Days</t>
-  </si>
-  <si>
     <t>522</t>
-  </si>
-  <si>
-    <t>74312004902</t>
-  </si>
-  <si>
-    <t>LUTEIN 20MG SOFTGELS</t>
   </si>
   <si>
     <t>MEDICARE A PER DIEM</t>
@@ -229,16 +163,7 @@
     <t>SANTYL       OIN 250/GM</t>
   </si>
   <si>
-    <t>TEHNNDER, CHRNSTNNE</t>
-  </si>
-  <si>
-    <t>TCSHNNE, WNHHNNT</t>
-  </si>
-  <si>
     <t>CNRROHH, BNRBNRN</t>
-  </si>
-  <si>
-    <t>TCNOVERN, FRNNK</t>
   </si>
   <si>
     <t>BUNNY, TNRNUERNTE</t>
@@ -254,9 +179,6 @@
   </si>
   <si>
     <t>7P34N88DT80</t>
-  </si>
-  <si>
-    <t>882228880T</t>
   </si>
 </sst>
 </file>
@@ -626,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -640,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:W264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -652,6 +574,8 @@
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -680,7 +604,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -730,13 +654,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2">
         <v>14856</v>
@@ -748,16 +672,16 @@
         <v>44067</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="L2" s="3">
         <v>44104</v>
@@ -766,28 +690,28 @@
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="4">
         <v>14</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="T2" s="6">
         <v>126</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,13 +719,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2">
         <v>14856</v>
@@ -813,16 +737,16 @@
         <v>44067</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="3">
         <v>44077</v>
@@ -831,10 +755,10 @@
         <v>16055356</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="P3" s="5">
         <v>0</v>
@@ -843,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="S3" s="4">
         <v>14</v>
@@ -852,13 +776,13 @@
         <v>21.42</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -866,13 +790,13 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
         <v>13003</v>
@@ -884,16 +808,16 @@
         <v>44083</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="L4" s="3">
         <v>44104</v>
@@ -902,28 +826,28 @@
         <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="4">
         <v>22</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="T4" s="6">
         <v>198</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -931,13 +855,13 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2">
         <v>17805</v>
@@ -949,16 +873,16 @@
         <v>44089</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="L5" s="3">
         <v>44104</v>
@@ -967,28 +891,28 @@
         <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="4">
         <v>16</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="T5" s="6">
         <v>144</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,13 +920,13 @@
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2">
         <v>17805</v>
@@ -1014,16 +938,16 @@
         <v>44089</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="L6" s="3">
         <v>44089</v>
@@ -1032,10 +956,10 @@
         <v>16142586</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="P6" s="5">
         <v>0</v>
@@ -1044,7 +968,7 @@
         <v>30</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="S6" s="4">
         <v>3</v>
@@ -1053,641 +977,235 @@
         <v>252.79</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2">
-        <v>17805</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="3">
-        <v>44089</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3">
-        <v>44092</v>
-      </c>
-      <c r="M7" s="4">
-        <v>16171681</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>30</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S7" s="4">
-        <v>3</v>
-      </c>
-      <c r="T7" s="6">
-        <v>252.79</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2">
-        <v>17805</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="3">
-        <v>44089</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="3">
-        <v>44098</v>
-      </c>
-      <c r="M8" s="4">
-        <v>16210280</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>30</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S8" s="4">
-        <v>3</v>
-      </c>
-      <c r="T8" s="6">
-        <v>252.79</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
     </row>
     <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2">
-        <v>11442</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="3">
-        <v>44111</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="3">
-        <v>44075</v>
-      </c>
-      <c r="M9" s="4">
-        <v>16039596</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>30</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S9" s="4">
-        <v>30</v>
-      </c>
-      <c r="T9" s="6">
-        <v>21.49</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
     </row>
     <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2">
-        <v>11442</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="3">
-        <v>44111</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="3">
-        <v>44104</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>24</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T10" s="6">
-        <v>216</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="1"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
     </row>
     <row r="11" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="2">
-        <v>11442</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="3">
-        <v>44111</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="3">
-        <v>44075</v>
-      </c>
-      <c r="M11" s="4">
-        <v>16039594</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>14</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S11" s="4">
-        <v>14</v>
-      </c>
-      <c r="T11" s="6">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
     </row>
     <row r="12" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2">
-        <v>9946</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="3">
-        <v>44096</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="3">
-        <v>44097</v>
-      </c>
-      <c r="M12" s="4">
-        <v>16200618</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P12" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>3</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S12" s="4">
-        <v>3</v>
-      </c>
-      <c r="T12" s="6">
-        <v>37.79</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="2">
-        <v>9946</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="3">
-        <v>44096</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="3">
-        <v>44099</v>
-      </c>
-      <c r="M13" s="4">
-        <v>16214527</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>14</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S13" s="4">
-        <v>14</v>
-      </c>
-      <c r="T13" s="6">
-        <v>169.02</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2">
-        <v>9946</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="3">
-        <v>44096</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="3">
-        <v>44104</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>9</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T14" s="6">
-        <v>81</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="1"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
     </row>
     <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2">
-        <v>22303</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="3">
-        <v>44096</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L15" s="3">
-        <v>44100</v>
-      </c>
-      <c r="M15" s="4">
-        <v>16228468</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>28</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S15" s="4">
-        <v>14</v>
-      </c>
-      <c r="T15" s="6">
-        <v>19.54</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
     </row>
     <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>

</xml_diff>